<commit_message>
Corrección en el error del campo id y en la visualización de los resultados
Para corregir la generación automática del campo id, se elimino este campo de la descripciones importada de las tablas en el script models.py
En el caso de la corrección de la visualización de los resultados, se actualizo los nombres de los campos que contenían mayúsculas a minúsculas, que corresponde a la redefinición de la nueva descripción, ya que los campos que contenían mayúsculas , generaban errores al ser importados del proyecto origen, al proyecto destino.
</commit_message>
<xml_diff>
--- a/Deltares.xlsx
+++ b/Deltares.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Deltares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4312D37-3C70-42C2-9C50-5EBD31D0706F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C64BEE-F82F-4308-A5E8-7F1D541D9A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{7BAE2FE5-DF0F-4ACF-9C1A-C0AE2684CAB4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BAE2FE5-DF0F-4ACF-9C1A-C0AE2684CAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Proceso de instalación" sheetId="27" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Descripción</t>
   </si>
@@ -122,9 +122,6 @@
     <t>pip install requests</t>
   </si>
   <si>
-    <t>GDAL_LIBRARY_PATH = r'C:\Users\Usuario\anaconda3\envs\deltaresEnv\Library\bin\gdal.dll'</t>
-  </si>
-  <si>
     <t>En el archivo settings, modificar la siguiente línea</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Pasos a seguir para instalar el proyecto P001_PostGis</t>
   </si>
   <si>
-    <t>Crear la base de datos Deltares2 en pgAdmin.</t>
-  </si>
-  <si>
     <t>clonar repositorio Git de Github</t>
   </si>
   <si>
@@ -240,6 +234,18 @@
   </si>
   <si>
     <t>python Deltares_GPP_Service.py</t>
+  </si>
+  <si>
+    <t>Crear la base de datos Deltares en pgAdmin.</t>
+  </si>
+  <si>
+    <t>GDAL_LIBRARY_PATH = r'C:\Users\Usuario\anaconda3\envs\PostGisEnv\Library\bin\gdal.dll'</t>
+  </si>
+  <si>
+    <t>el usuario y el password: mfuentes Y2k260599</t>
+  </si>
+  <si>
+    <t>pip install crispy-bootstrap4</t>
   </si>
 </sst>
 </file>
@@ -636,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDB68E5-E50E-4923-ACB8-BAF83A53D523}">
-  <dimension ref="A1:A104"/>
+  <dimension ref="A1:A86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:XFD109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +660,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -689,12 +695,12 @@
     </row>
     <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -704,27 +710,27 @@
     </row>
     <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -744,37 +750,37 @@
     </row>
     <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -819,7 +825,7 @@
     </row>
     <row r="35" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -829,32 +835,32 @@
     </row>
     <row r="37" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -889,192 +895,192 @@
     </row>
     <row r="49" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
+    <row r="58" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+    <row r="61" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+    <row r="62" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:1" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
-        <v>46</v>
+    <row r="67" spans="1:1" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="84" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>7</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Libro de Excel con la configuración de la instalación
Libro de Excel con la configuración de la instalación, de los tres proyectos de django, base de datos, página web y servicio
</commit_message>
<xml_diff>
--- a/Deltares.xlsx
+++ b/Deltares.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Deltares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C64BEE-F82F-4308-A5E8-7F1D541D9A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF8292-F3B1-4C1E-83FF-993617400F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BAE2FE5-DF0F-4ACF-9C1A-C0AE2684CAB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{7BAE2FE5-DF0F-4ACF-9C1A-C0AE2684CAB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Proceso de instalación" sheetId="27" r:id="rId1"/>
@@ -644,441 +644,441 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDB68E5-E50E-4923-ACB8-BAF83A53D523}">
   <dimension ref="A1:A86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A104" sqref="A104:XFD109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="126.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="126.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:1" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:1" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>65</v>
       </c>

</xml_diff>